<commit_message>
formula: support for more math/trig formulas
- EVEN
- EXP
- FACT
- FACTDOUBLE
- FLOOR.MATH
- FLOOR.PRECISE
- GCD
- INT
- ISO.CEILING
- LCM
- LN
- LOG
- LOG10
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -124,6 +124,45 @@
   </si>
   <si>
     <t xml:space="preserve">DEGREES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACTDOUBLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOOR.MATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOOR.PRECISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO.CEILING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOG10</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -325,9 +364,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,9 +436,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,25 +886,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:T46"/>
+  <dimension ref="A2:AG46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG7" activeCellId="0" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -925,6 +967,45 @@
       <c r="T2" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1000,6 +1081,58 @@
       </c>
       <c r="T3" s="0" t="e">
         <f aca="false">DEGREES()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U3" s="0" t="e">
+        <f aca="false">EVEN()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V3" s="0" t="e">
+        <f aca="false">EXP(U3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W3" s="0" t="e">
+        <f aca="false">FACT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X3" s="0" t="e">
+        <f aca="false">FACTDOUBLE()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y3" s="0" t="e">
+        <f aca="false">_xlfn.FLOOR.MATH()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z3" s="0" t="e">
+        <f aca="false">_xlfn.FLOOR.PRECISE()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AA3" s="0" t="e">
+        <f aca="false">GCD()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB3" s="0" t="e">
+        <f aca="false">INT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC3" s="0" t="e">
+        <f aca="false">ISO.CEILING()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD3" s="0" t="e">
+        <f aca="false">LCM()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AE3" s="0" t="e">
+        <f aca="false">LN()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF3" s="0" t="e">
+        <f aca="false">LOG()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG3" s="0" t="e">
+        <f aca="false">LOG10()</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1079,6 +1212,58 @@
         <f aca="false">DEGREES(0)</f>
         <v>0</v>
       </c>
+      <c r="U4" s="0" t="n">
+        <f aca="false">EVEN(1.6)</f>
+        <v>2</v>
+      </c>
+      <c r="V4" s="0" t="e">
+        <f aca="false">EXP()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W4" s="0" t="e">
+        <f aca="false">FACT(-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <f aca="false">FACTDOUBLE(0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(3.7,2)</f>
+        <v>2</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.PRECISE(-3.2,-1)</f>
+        <v>-4</v>
+      </c>
+      <c r="AA4" s="0" t="e">
+        <f aca="false">GCD(Z4:Z7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <f aca="false">INT(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <f aca="false">ISO.CEILING(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="0" t="n">
+        <f aca="false">LCM(5,2)</f>
+        <v>10</v>
+      </c>
+      <c r="AE4" s="0" t="str">
+        <f aca="false">LEFT(LN(86),5)</f>
+        <v>4.454</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <f aca="false">LOG(10)</f>
+        <v>1</v>
+      </c>
+      <c r="AG4" s="0" t="n">
+        <f aca="false">LOG10(100)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1157,6 +1342,58 @@
         <f aca="false">DEGREES(-PI())</f>
         <v>-180</v>
       </c>
+      <c r="U5" s="0" t="n">
+        <f aca="false">EVEN(3)</f>
+        <v>4</v>
+      </c>
+      <c r="V5" s="0" t="str">
+        <f aca="false">LEFT(EXP(U5),5)</f>
+        <v>54.59</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <f aca="false">FACT(0)</f>
+        <v>1</v>
+      </c>
+      <c r="X5" s="0" t="e">
+        <f aca="false">FACTDOUBLE(-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(-2.5,-2)</f>
+        <v>-4</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.PRECISE(3.2,1)</f>
+        <v>3</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <f aca="false">GCD(Y6:Y8)</f>
+        <v>1</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <f aca="false">INT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <f aca="false">ISO.CEILING(4.3)</f>
+        <v>5</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <f aca="false">LCM(24,36)</f>
+        <v>72</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <f aca="false">LN(EXP(3.15))</f>
+        <v>3.15</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <f aca="false">LOG(8,2)</f>
+        <v>3</v>
+      </c>
+      <c r="AG5" s="0" t="e">
+        <f aca="false">LOG10(0)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1227,6 +1464,58 @@
         <f aca="false">DEGREES(PI())</f>
         <v>180</v>
       </c>
+      <c r="U6" s="0" t="n">
+        <f aca="false">EVEN(2)</f>
+        <v>2</v>
+      </c>
+      <c r="V6" s="0" t="str">
+        <f aca="false">LEFT(EXP(U7),5)</f>
+        <v>0.135</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <f aca="false">FACT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <f aca="false">FACTDOUBLE(6)</f>
+        <v>48</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(2.5,-2)</f>
+        <v>2</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.PRECISE(-3.2,1)</f>
+        <v>-4</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <f aca="false">GCD(5,2)</f>
+        <v>1</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <f aca="false">INT(8.9)</f>
+        <v>8</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <f aca="false">ISO.CEILING(-4.3)</f>
+        <v>-4</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <f aca="false">LCM(1,2,3,5)</f>
+        <v>30</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <f aca="false">LN(EXP(3))</f>
+        <v>3</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <f aca="false">LOG(1024,2)</f>
+        <v>10</v>
+      </c>
+      <c r="AG6" s="0" t="n">
+        <f aca="false">LOG10(1000)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1293,6 +1582,46 @@
         <f aca="false">_xlfn.DECIMAL(100,5)</f>
         <v>25</v>
       </c>
+      <c r="U7" s="0" t="n">
+        <f aca="false">EVEN(-1)</f>
+        <v>-2</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <f aca="false">FACT(5)</f>
+        <v>120</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <f aca="false">FACTDOUBLE(7)</f>
+        <v>105</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(1.58,0.1)</f>
+        <v>1.5</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.PRECISE(3.2,-1)</f>
+        <v>3</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <f aca="false">GCD(24,36)</f>
+        <v>12</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <f aca="false">INT(-8.9)</f>
+        <v>-9</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <f aca="false">ISO.CEILING(4.3,2)</f>
+        <v>6</v>
+      </c>
+      <c r="AD7" s="0" t="n">
+        <f aca="false">LCM(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="0" t="e">
+        <f aca="false">LOG(0)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1355,6 +1684,38 @@
         <f aca="false">_xlfn.COMBINA(5,3)</f>
         <v>35</v>
       </c>
+      <c r="U8" s="0" t="e">
+        <f aca="false">EVEN(U6:U7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(0.234,0.01)</f>
+        <v>0.23</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.PRECISE(3.2)</f>
+        <v>3</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <f aca="false">GCD(7,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <f aca="false">INT(0.5)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <f aca="false">ISO.CEILING(4.3,-2)</f>
+        <v>6</v>
+      </c>
+      <c r="AD8" s="0" t="e">
+        <f aca="false">LCM(-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF8" s="0" t="e">
+        <f aca="false">LOG(10,0)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1392,6 +1753,30 @@
         <f aca="false">_xlfn.COMBINA(5,0)</f>
         <v>1</v>
       </c>
+      <c r="Y9" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(1.5)</f>
+        <v>1</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <f aca="false">GCD(5,0)</f>
+        <v>5</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <f aca="false">INT(-0.5)</f>
+        <v>-1</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <f aca="false">ISO.CEILING(-4.3,2)</f>
+        <v>-4</v>
+      </c>
+      <c r="AD9" s="0" t="e">
+        <f aca="false">LCM(5,2,-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF9" s="0" t="e">
+        <f aca="false">LOG(1,0)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -1421,6 +1806,26 @@
         <f aca="false">_xlfn.COMBINA(0,5)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="Y10" s="0" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH(-1.5)</f>
+        <v>-2</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <f aca="false">GCD(5)</f>
+        <v>5</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <f aca="false">INT(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <f aca="false">ISO.CEILING(-4.3,-2)</f>
+        <v>-4</v>
+      </c>
+      <c r="AD10" s="0" t="n">
+        <f aca="false">LCM(5,23,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -1437,6 +1842,14 @@
       <c r="M11" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(-8.1,2)</f>
         <v>-8</v>
+      </c>
+      <c r="AA11" s="0" t="e">
+        <f aca="false">GCD(5,8,"a")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD11" s="0" t="n">
+        <f aca="false">LCM(0,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1456,16 +1869,28 @@
         <f aca="false">_xlfn.CEILING.MATH(-5.5,2,-1)</f>
         <v>-6</v>
       </c>
+      <c r="AA12" s="0" t="n">
+        <f aca="false">GCD(2,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="AA13" s="0" t="n">
+        <f aca="false">GCD(0,5)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="AA14" s="0" t="n">
+        <f aca="false">GCD(0,0,6)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1484,42 +1909,42 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A26)</f>
@@ -1528,7 +1953,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A27)</f>
@@ -1537,7 +1962,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A28)</f>
@@ -1546,7 +1971,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A29)</f>
@@ -1555,7 +1980,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A30)</f>
@@ -1564,7 +1989,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A31)</f>
@@ -1573,7 +1998,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A33)</f>
@@ -1582,7 +2007,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A34)</f>
@@ -1591,7 +2016,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A35)</f>
@@ -1600,7 +2025,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A36)</f>
@@ -1609,7 +2034,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A37)</f>
@@ -1618,7 +2043,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A38)</f>
@@ -1627,7 +2052,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A39)</f>
@@ -1636,7 +2061,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F41" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A41)</f>
@@ -1645,7 +2070,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F42" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A42)</f>
@@ -1654,7 +2079,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A43)</f>
@@ -1663,7 +2088,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A44)</f>
@@ -1672,7 +2097,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A45)</f>
@@ -1681,7 +2106,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A46)</f>

</xml_diff>

<commit_message>
formula: add support for referencing other sheets
This adds support references like 'Sheet 1'! so that formulas
can pull values from other sheets.
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve">Divide by Zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference Other Sheet</t>
   </si>
   <si>
     <t xml:space="preserve">AND</t>
@@ -356,17 +359,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,6 +412,19 @@
       <c r="E8" s="0" t="e">
         <f aca="false">C8/D8</f>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">Logical!A3</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">'Math and Trig'!N7</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -436,37 +451,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,7 +724,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="e">
         <f aca="false">AND(A10:A11)</f>
@@ -735,7 +749,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="e">
         <f aca="false">AND()</f>
@@ -774,7 +788,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="0" t="e">
         <f aca="false">IF(A9,A10,A11,A8)</f>
@@ -787,7 +801,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="0" t="e">
         <f aca="false">IF(A11,TRUE())</f>
@@ -800,7 +814,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I15" s="3" t="e">
         <f aca="false">_xlfn.XOR(A10:A11)</f>
@@ -888,123 +902,124 @@
   </sheetPr>
   <dimension ref="A2:AG46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AG7" activeCellId="0" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1795,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="e">
         <f aca="false">ABS(A7:A9)</f>
@@ -1829,7 +1844,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A23)</f>
@@ -1876,7 +1891,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA13" s="0" t="n">
         <f aca="false">GCD(0,5)</f>
@@ -1885,7 +1900,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA14" s="0" t="n">
         <f aca="false">GCD(0,0,6)</f>
@@ -1894,7 +1909,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,42 +1924,42 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A26)</f>
@@ -1953,7 +1968,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A27)</f>
@@ -1962,7 +1977,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A28)</f>
@@ -1971,7 +1986,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A29)</f>
@@ -1980,7 +1995,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A30)</f>
@@ -1989,7 +2004,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A31)</f>
@@ -1998,7 +2013,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A33)</f>
@@ -2007,7 +2022,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A34)</f>
@@ -2016,7 +2031,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A35)</f>
@@ -2025,7 +2040,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A36)</f>
@@ -2034,7 +2049,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A37)</f>
@@ -2043,7 +2058,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A38)</f>
@@ -2052,7 +2067,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A39)</f>
@@ -2061,7 +2076,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F41" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A41)</f>
@@ -2070,7 +2085,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F42" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A42)</f>
@@ -2079,7 +2094,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A43)</f>
@@ -2088,7 +2103,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A44)</f>
@@ -2097,7 +2112,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A45)</f>
@@ -2106,7 +2121,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A46)</f>

</xml_diff>

<commit_message>
formula: add initial support for cell arrays
This is a pretty uncommon feature from what I can tell
and is not fully supported. The example for the MDETERM
function uses an array though, so this will at least add
enough support for the examples to compute correctly.
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reference Other Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Const Array</t>
   </si>
   <si>
     <t xml:space="preserve">AND</t>
@@ -322,6 +325,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,10 +343,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -359,16 +362,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,6 +430,61 @@
       <c r="E10" s="0" t="n">
         <f aca="false">'Math and Trig'!N7</f>
         <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">SUM({1;2})</f>
+        <v>3</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <f aca="false">SUM({1,1,1})</f>
+        <v>3</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <f aca="false">SUM({1;3;5})</f>
+        <v>9</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false" t="array" ref="D15:F15">D13:F13*D14:F14</f>
+        <v>4</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="n">
+        <f aca="false">SUM({3,4,5,6,7}*{1,2,3,4,5})</f>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -451,36 +511,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,7 +783,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="e">
         <f aca="false">AND(A10:A11)</f>
@@ -749,7 +808,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="e">
         <f aca="false">AND()</f>
@@ -788,7 +847,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" s="0" t="e">
         <f aca="false">IF(A9,A10,A11,A8)</f>
@@ -801,7 +860,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" s="0" t="e">
         <f aca="false">IF(A11,TRUE())</f>
@@ -814,9 +873,9 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="3" t="e">
+        <v>16</v>
+      </c>
+      <c r="I15" s="4" t="e">
         <f aca="false">_xlfn.XOR(A10:A11)</f>
         <v>#VALUE!</v>
       </c>
@@ -825,7 +884,7 @@
       <c r="A16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="4" t="n">
         <f aca="false">_xlfn.XOR(A9:A11)</f>
         <v>1</v>
       </c>
@@ -908,118 +967,113 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="R2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="U2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="V2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="W2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="X2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Y2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="Z2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AA2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AB2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AC2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AD2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AE2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AF2" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,7 +1253,7 @@
         <f aca="false">_xlfn.CEILING.MATH(K4)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N4" s="4" t="e">
+      <c r="N4" s="5" t="e">
         <f aca="false">_xlfn.CEILING.PRECISE(M4)</f>
         <v>#VALUE!</v>
       </c>
@@ -1459,7 +1513,7 @@
         <f aca="false">_xlfn.CEILING.MATH(4.42,0.05)</f>
         <v>4.45</v>
       </c>
-      <c r="N6" s="4" t="n">
+      <c r="N6" s="5" t="n">
         <f aca="false">_xlfn.CEILING.PRECISE(-4.3)</f>
         <v>-4</v>
       </c>
@@ -1581,7 +1635,7 @@
         <f aca="false">_xlfn.CEILING.MATH(4.42,1)</f>
         <v>5</v>
       </c>
-      <c r="N7" s="4" t="n">
+      <c r="N7" s="5" t="n">
         <f aca="false">_xlfn.CEILING.PRECISE(4.3,2)</f>
         <v>6</v>
       </c>
@@ -1687,7 +1741,7 @@
         <f aca="false">_xlfn.CEILING.MATH(4.42,0.01)</f>
         <v>4.42</v>
       </c>
-      <c r="N8" s="4" t="n">
+      <c r="N8" s="5" t="n">
         <f aca="false">_xlfn.CEILING.PRECISE(4.3,-2)</f>
         <v>6</v>
       </c>
@@ -1756,7 +1810,7 @@
         <f aca="false">_xlfn.CEILING.MATH(24.3,5)</f>
         <v>25</v>
       </c>
-      <c r="N9" s="4" t="n">
+      <c r="N9" s="5" t="n">
         <f aca="false">_xlfn.CEILING.PRECISE(-4.3,2)</f>
         <v>-4</v>
       </c>
@@ -1795,7 +1849,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="e">
         <f aca="false">ABS(A7:A9)</f>
@@ -1813,7 +1867,7 @@
         <f aca="false">_xlfn.CEILING.MATH(6.7)</f>
         <v>7</v>
       </c>
-      <c r="N10" s="4" t="n">
+      <c r="N10" s="5" t="n">
         <f aca="false">_xlfn.CEILING.PRECISE(-4.3,-2)</f>
         <v>-4</v>
       </c>
@@ -1844,7 +1898,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A23)</f>
@@ -1891,7 +1945,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AA13" s="0" t="n">
         <f aca="false">GCD(0,5)</f>
@@ -1900,7 +1954,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AA14" s="0" t="n">
         <f aca="false">GCD(0,0,6)</f>
@@ -1909,7 +1963,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,42 +1978,42 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>54</v>
+      <c r="A24" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A26)</f>
@@ -1968,7 +2022,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A27)</f>
@@ -1977,7 +2031,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A28)</f>
@@ -1986,7 +2040,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A29)</f>
@@ -1995,7 +2049,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A30)</f>
@@ -2004,7 +2058,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A31)</f>
@@ -2013,7 +2067,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A33)</f>
@@ -2022,7 +2076,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A34)</f>
@@ -2031,7 +2085,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A35)</f>
@@ -2040,7 +2094,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A36)</f>
@@ -2049,7 +2103,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A37)</f>
@@ -2058,7 +2112,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A38)</f>
@@ -2067,7 +2121,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A39)</f>
@@ -2076,7 +2130,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F41" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A41)</f>
@@ -2085,7 +2139,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F42" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A42)</f>
@@ -2094,7 +2148,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A43)</f>
@@ -2103,7 +2157,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A44)</f>
@@ -2112,7 +2166,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A45)</f>
@@ -2121,7 +2175,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A46)</f>

</xml_diff>

<commit_message>
formula: more implementations of math/trig functins
- MDETERM
- MOD
- MROUND
- MULTINOMIAL
- MUNIT
- ODD
- POWER
- PRODUCT
- QUOTIENT
- RADIANS
- RAND
- RANDBETWEEN
- ROMAN
- ROUND
- ROUNDDOWN
- ROUNDUP
- SERIESSUM
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">Recursive formula</t>
   </si>
   <si>
+    <t xml:space="preserve">Exponent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Divide by Zero</t>
   </si>
   <si>
@@ -169,6 +172,51 @@
   </si>
   <si>
     <t xml:space="preserve">LOG10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDETERM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTINOMIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUNIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUOTIENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RADIANS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROMAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROUNDDOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROUNDUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERIESSUM</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -362,18 +410,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,10 +449,17 @@
         <f aca="false">C7</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">5^2</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>5</v>
@@ -421,7 +474,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">Logical!A3</f>
@@ -434,7 +487,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">SUM({1;2})</f>
@@ -511,35 +564,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +837,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="e">
         <f aca="false">AND(A10:A11)</f>
@@ -808,7 +862,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="e">
         <f aca="false">AND()</f>
@@ -847,7 +901,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="e">
         <f aca="false">IF(A9,A10,A11,A8)</f>
@@ -860,7 +914,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="0" t="e">
         <f aca="false">IF(A11,TRUE())</f>
@@ -873,7 +927,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="4" t="e">
         <f aca="false">_xlfn.XOR(A10:A11)</f>
@@ -959,121 +1013,182 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AG46"/>
+  <dimension ref="A1:AV46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG7" activeCellId="0" sqref="AG7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AV23" activeCellId="0" sqref="AV23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="40" min="38" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP1" s="2"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,6 +1318,62 @@
       <c r="AG3" s="0" t="e">
         <f aca="false">LOG10()</f>
         <v>#VALUE!</v>
+      </c>
+      <c r="AH3" s="0" t="e">
+        <f aca="false">MDETERM()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI3" s="0" t="e">
+        <f aca="false">MOD()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ3" s="0" t="e">
+        <f aca="false">MROUND()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK3" s="0" t="e">
+        <f aca="false">MULTINOMIAL()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL3" s="0" t="e">
+        <f aca="false">_xlfn.MUNIT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM3" s="0" t="e">
+        <f aca="false">ODD()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN3" s="0" t="e">
+        <f aca="false">POWER()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP3" s="0" t="e">
+        <f aca="false">QUOTIENT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <f aca="false">RADIANS(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AR3" s="0" t="str">
+        <f aca="false">ROMAN(499)</f>
+        <v>CDXCIX</v>
+      </c>
+      <c r="AS3" s="0" t="e">
+        <f aca="false">ROUND("A",0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT3" s="0" t="e">
+        <f aca="false">ROUNDDOWN("A",0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU3" s="0" t="e">
+        <f aca="false">ROUNDUP("A",0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AV3" s="0" t="str">
+        <f aca="false">LEFT(SERIESSUM(AV18,0,2,AV19:AV22),7)</f>
+        <v>0.69158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,6 +1504,62 @@
         <f aca="false">LOG10(100)</f>
         <v>2</v>
       </c>
+      <c r="AH4" s="0" t="e">
+        <f aca="false">MDETERM({1,3,8,5;1,3,6,1})</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI4" s="0" t="e">
+        <f aca="false">MOD(1.2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AJ4" s="0" t="n">
+        <f aca="false">MROUND(10,3)</f>
+        <v>9</v>
+      </c>
+      <c r="AK4" s="0" t="n">
+        <f aca="false">MULTINOMIAL(0)</f>
+        <v>1</v>
+      </c>
+      <c r="AL4" s="0" t="n">
+        <f aca="false">_xlfn.MUNIT(2)</f>
+        <v>1</v>
+      </c>
+      <c r="AM4" s="0" t="n">
+        <f aca="false">ODD(1.5)</f>
+        <v>3</v>
+      </c>
+      <c r="AN4" s="0" t="n">
+        <f aca="false">POWER(0,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO4" s="0" t="n">
+        <f aca="false">PRODUCT(2)</f>
+        <v>2</v>
+      </c>
+      <c r="AP4" s="0" t="n">
+        <f aca="false">QUOTIENT(5,2)</f>
+        <v>2</v>
+      </c>
+      <c r="AQ4" s="0" t="n">
+        <f aca="false">DEGREES(RADIANS(180))</f>
+        <v>180</v>
+      </c>
+      <c r="AR4" s="0" t="str">
+        <f aca="false">ROMAN(499,0)</f>
+        <v>CDXCIX</v>
+      </c>
+      <c r="AS4" s="0" t="n">
+        <f aca="false">ROUND(2.15,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AT4" s="0" t="n">
+        <f aca="false">ROUNDDOWN(2.15,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AU4" s="0" t="n">
+        <f aca="false">ROUNDUP(2.15,0)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1463,6 +1690,62 @@
         <f aca="false">LOG10(0)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AH5" s="0" t="n">
+        <f aca="false">MDETERM({3,6,1;1,1,0;3,10,2})</f>
+        <v>1</v>
+      </c>
+      <c r="AI5" s="0" t="n">
+        <f aca="false">MOD(1.2,4)</f>
+        <v>1.2</v>
+      </c>
+      <c r="AJ5" s="0" t="n">
+        <f aca="false">MROUND(-10,-3)</f>
+        <v>-9</v>
+      </c>
+      <c r="AK5" s="0" t="n">
+        <f aca="false">MULTINOMIAL(1,2,3)</f>
+        <v>60</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <f aca="false">_xlfn.MUNIT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <f aca="false">ODD(3)</f>
+        <v>3</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <f aca="false">POWER(1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO5" s="0" t="n">
+        <f aca="false">PRODUCT(AN4:AN8)</f>
+        <v>-1024</v>
+      </c>
+      <c r="AP5" s="0" t="n">
+        <f aca="false">QUOTIENT(4.5,3.1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="0" t="n">
+        <f aca="false">DEGREES(RADIANS(45))</f>
+        <v>45</v>
+      </c>
+      <c r="AR5" s="0" t="str">
+        <f aca="false">ROMAN(499,1)</f>
+        <v>LDVLIV</v>
+      </c>
+      <c r="AS5" s="0" t="n">
+        <f aca="false">ROUND(2.15,1)</f>
+        <v>2.2</v>
+      </c>
+      <c r="AT5" s="0" t="n">
+        <f aca="false">ROUNDDOWN(2.15,1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="AU5" s="0" t="n">
+        <f aca="false">ROUNDUP(2.15,1)</f>
+        <v>2.2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1585,6 +1868,58 @@
         <f aca="false">LOG10(1000)</f>
         <v>3</v>
       </c>
+      <c r="AH6" s="1" t="n">
+        <f aca="false">MDETERM({3,6;1,1})</f>
+        <v>-3</v>
+      </c>
+      <c r="AI6" s="1" t="n">
+        <f aca="false">MOD(5,3)</f>
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="0" t="n">
+        <f aca="false">MROUND(1.3,0.2)</f>
+        <v>1.4</v>
+      </c>
+      <c r="AK6" s="0" t="n">
+        <f aca="false">MULTINOMIAL(4,5,6)</f>
+        <v>630630</v>
+      </c>
+      <c r="AL6" s="0" t="e">
+        <f aca="false">_xlfn.MUNIT(AK2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM6" s="0" t="n">
+        <f aca="false">ODD(2)</f>
+        <v>3</v>
+      </c>
+      <c r="AN6" s="0" t="n">
+        <f aca="false">POWER(-1,5)</f>
+        <v>-1</v>
+      </c>
+      <c r="AO6" s="0" t="n">
+        <f aca="false">PRODUCT(AM4:AM8)</f>
+        <v>81</v>
+      </c>
+      <c r="AP6" s="0" t="n">
+        <f aca="false">QUOTIENT(-10,3)</f>
+        <v>-3</v>
+      </c>
+      <c r="AR6" s="0" t="str">
+        <f aca="false">ROMAN(499,2)</f>
+        <v>XDIX</v>
+      </c>
+      <c r="AS6" s="0" t="n">
+        <f aca="false">ROUND(2.149,1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="AT6" s="0" t="n">
+        <f aca="false">ROUNDDOWN(2.149,1)</f>
+        <v>2.1</v>
+      </c>
+      <c r="AU6" s="0" t="n">
+        <f aca="false">ROUNDUP(2.149,1)</f>
+        <v>2.2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1691,6 +2026,50 @@
         <f aca="false">LOG(0)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AH7" s="0" t="n">
+        <f aca="false">MDETERM({1,2,3;0,-4,1;0,3,-1})</f>
+        <v>1</v>
+      </c>
+      <c r="AI7" s="0" t="n">
+        <f aca="false">MOD(3,2)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="0" t="e">
+        <f aca="false">MROUND(1.4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK7" s="0" t="n">
+        <f aca="false">MULTINOMIAL(AI6:AI8)</f>
+        <v>12</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <f aca="false">_xlfn.MUNIT(4)</f>
+        <v>1</v>
+      </c>
+      <c r="AM7" s="0" t="n">
+        <f aca="false">ODD(-1)</f>
+        <v>-1</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <f aca="false">POWER(-1,4)</f>
+        <v>1</v>
+      </c>
+      <c r="AR7" s="0" t="str">
+        <f aca="false">ROMAN(499,3)</f>
+        <v>VDIV</v>
+      </c>
+      <c r="AS7" s="0" t="n">
+        <f aca="false">ROUND(-1.475,2)</f>
+        <v>-1.48</v>
+      </c>
+      <c r="AT7" s="0" t="n">
+        <f aca="false">ROUNDDOWN(-1.475,2)</f>
+        <v>-1.47</v>
+      </c>
+      <c r="AU7" s="0" t="n">
+        <f aca="false">ROUNDUP(-1.475,2)</f>
+        <v>-1.48</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1785,6 +2164,42 @@
         <f aca="false">LOG(10,0)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AH8" s="5" t="n">
+        <f aca="false">MDETERM({1,2,3,4,5;6,1,5,6,3;1,9,4,1,6;1,4,7,9,3;1,65,8,2,1})</f>
+        <v>28310</v>
+      </c>
+      <c r="AI8" s="5" t="n">
+        <f aca="false">MOD(-3,2)</f>
+        <v>1</v>
+      </c>
+      <c r="AK8" s="0" t="n">
+        <f aca="false">MULTINOMIAL(1.5,3.4)</f>
+        <v>4</v>
+      </c>
+      <c r="AM8" s="0" t="n">
+        <f aca="false">ODD(-2)</f>
+        <v>-3</v>
+      </c>
+      <c r="AN8" s="0" t="n">
+        <f aca="false">POWER(2,10)</f>
+        <v>1024</v>
+      </c>
+      <c r="AR8" s="0" t="str">
+        <f aca="false">ROMAN(499,4)</f>
+        <v>ID</v>
+      </c>
+      <c r="AS8" s="0" t="n">
+        <f aca="false">ROUND(21.5,-1)</f>
+        <v>20</v>
+      </c>
+      <c r="AT8" s="0" t="n">
+        <f aca="false">ROUNDDOWN(21.5,-1)</f>
+        <v>20</v>
+      </c>
+      <c r="AU8" s="0" t="n">
+        <f aca="false">ROUNDUP(21.5,-1)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1846,10 +2261,38 @@
         <f aca="false">LOG(1,0)</f>
         <v>#VALUE!</v>
       </c>
+      <c r="AI9" s="0" t="n">
+        <f aca="false">MOD(3,-2)</f>
+        <v>-1</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <f aca="false">MULTINOMIAL(AI6:AI8,AI6:AI8)</f>
+        <v>10080</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <f aca="false">POWER(1.5,3)</f>
+        <v>3.375</v>
+      </c>
+      <c r="AR9" s="0" t="str">
+        <f aca="false">ROMAN(99,0)</f>
+        <v>XCIX</v>
+      </c>
+      <c r="AS9" s="0" t="n">
+        <f aca="false">ROUND(626.3,-3)</f>
+        <v>1000</v>
+      </c>
+      <c r="AT9" s="0" t="n">
+        <f aca="false">ROUNDDOWN(626.3,-3)</f>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="0" t="n">
+        <f aca="false">ROUNDUP(626.3,-3)</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="e">
         <f aca="false">ABS(A7:A9)</f>
@@ -1895,10 +2338,34 @@
         <f aca="false">LCM(5,23,0)</f>
         <v>0</v>
       </c>
+      <c r="AK10" s="0" t="n">
+        <f aca="false">MULTINOMIAL(1,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="AN10" s="0" t="e">
+        <f aca="false">POWER(5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR10" s="0" t="str">
+        <f aca="false">ROMAN(99,1)</f>
+        <v>VCIV</v>
+      </c>
+      <c r="AS10" s="0" t="n">
+        <f aca="false">ROUND(1.98,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="AT10" s="0" t="n">
+        <f aca="false">ROUNDDOWN(1.98,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="0" t="n">
+        <f aca="false">ROUNDUP(1.98,-1)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F11" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A23)</f>
@@ -1919,6 +2386,22 @@
       <c r="AD11" s="0" t="n">
         <f aca="false">LCM(0,0)</f>
         <v>0</v>
+      </c>
+      <c r="AR11" s="0" t="str">
+        <f aca="false">ROMAN(99,2)</f>
+        <v>IC</v>
+      </c>
+      <c r="AS11" s="0" t="n">
+        <f aca="false">ROUND(-50.55,-2)</f>
+        <v>-100</v>
+      </c>
+      <c r="AT11" s="0" t="n">
+        <f aca="false">ROUNDDOWN(-50.55,-2)</f>
+        <v>-0</v>
+      </c>
+      <c r="AU11" s="0" t="n">
+        <f aca="false">ROUNDUP(-50.55,-2)</f>
+        <v>-100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1942,78 +2425,201 @@
         <f aca="false">GCD(2,0)</f>
         <v>2</v>
       </c>
+      <c r="AR12" s="0" t="str">
+        <f aca="false">ROMAN(99,3)</f>
+        <v>IC</v>
+      </c>
+      <c r="AS12" s="0" t="n">
+        <f aca="false">ROUND(1.23,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AT12" s="0" t="n">
+        <f aca="false">ROUNDDOWN(1.23,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU12" s="0" t="n">
+        <f aca="false">ROUNDUP(1.23,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AA13" s="0" t="n">
         <f aca="false">GCD(0,5)</f>
         <v>5</v>
       </c>
+      <c r="AR13" s="0" t="str">
+        <f aca="false">ROMAN(99,4)</f>
+        <v>IC</v>
+      </c>
+      <c r="AS13" s="0" t="n">
+        <f aca="false">ROUND(1.49,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AT13" s="0" t="n">
+        <f aca="false">ROUNDDOWN(1.49,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU13" s="0" t="n">
+        <f aca="false">ROUNDUP(1.49,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AA14" s="0" t="n">
         <f aca="false">GCD(0,0,6)</f>
         <v>6</v>
       </c>
+      <c r="AR14" s="0" t="str">
+        <f aca="false">ROMAN(999)</f>
+        <v>CMXCIX</v>
+      </c>
+      <c r="AS14" s="0" t="n">
+        <f aca="false">ROUND(1.5,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AT14" s="0" t="n">
+        <f aca="false">ROUNDDOWN(1.5,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AU14" s="0" t="n">
+        <f aca="false">ROUNDUP(1.5,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="AR15" s="0" t="str">
+        <f aca="false">ROMAN(999,1)</f>
+        <v>LMVLIV</v>
+      </c>
+      <c r="AS15" s="0" t="n">
+        <f aca="false">ROUND(-1.49,0)</f>
+        <v>-1</v>
+      </c>
+      <c r="AT15" s="0" t="n">
+        <f aca="false">ROUNDDOWN(-1.49,0)</f>
+        <v>-1</v>
+      </c>
+      <c r="AU15" s="0" t="n">
+        <f aca="false">ROUNDUP(-1.49,0)</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="AR16" s="0" t="str">
+        <f aca="false">ROMAN(999,2)</f>
+        <v>XMIX</v>
+      </c>
+      <c r="AS16" s="0" t="n">
+        <f aca="false">ROUND(-1.5,0)</f>
+        <v>-2</v>
+      </c>
+      <c r="AT16" s="0" t="n">
+        <f aca="false">ROUNDDOWN(-1.5,0)</f>
+        <v>-1</v>
+      </c>
+      <c r="AU16" s="0" t="n">
+        <f aca="false">ROUNDUP(-1.5,0)</f>
+        <v>-2</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>-1.45</v>
       </c>
+      <c r="AR17" s="0" t="str">
+        <f aca="false">ROMAN(999,3)</f>
+        <v>VMIV</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
+      </c>
+      <c r="AR18" s="0" t="str">
+        <f aca="false">ROMAN(999,4)</f>
+        <v>IM</v>
+      </c>
+      <c r="AV18" s="0" t="str">
+        <f aca="false">LEFT(PI()/4,7)</f>
+        <v>0.78539</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
+      </c>
+      <c r="AR19" s="0" t="str">
+        <f aca="false">ROMAN(699,1)</f>
+        <v>DCVCIV</v>
+      </c>
+      <c r="AV19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
+      </c>
+      <c r="AR20" s="0" t="str">
+        <f aca="false">ROMAN(699,2)</f>
+        <v>DCIC</v>
+      </c>
+      <c r="AV20" s="0" t="n">
+        <f aca="false">-1/FACT(2)</f>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
+      </c>
+      <c r="AR21" s="0" t="str">
+        <f aca="false">ROMAN(699,3)</f>
+        <v>DCIC</v>
+      </c>
+      <c r="AV21" s="0" t="str">
+        <f aca="false">LEFT(1/FACT(4),7)</f>
+        <v>0.04166</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>53</v>
+        <v>69</v>
+      </c>
+      <c r="AR22" s="0" t="str">
+        <f aca="false">ROMAN(699,4)</f>
+        <v>DCIC</v>
+      </c>
+      <c r="AV22" s="0" t="str">
+        <f aca="false">LEFT(-1/FACT(6),7)</f>
+        <v>-0.0013</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A26)</f>
@@ -2022,7 +2628,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A27)</f>
@@ -2031,7 +2637,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A28)</f>
@@ -2040,7 +2646,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A29)</f>
@@ -2049,7 +2655,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A30)</f>
@@ -2058,7 +2664,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A31)</f>
@@ -2067,7 +2673,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A33)</f>
@@ -2076,7 +2682,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A34)</f>
@@ -2085,7 +2691,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A35)</f>
@@ -2094,7 +2700,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A36)</f>
@@ -2103,7 +2709,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A37)</f>
@@ -2112,7 +2718,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A38)</f>
@@ -2121,7 +2727,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A39)</f>
@@ -2130,7 +2736,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="F41" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A41)</f>
@@ -2139,7 +2745,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="F42" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A42)</f>
@@ -2148,7 +2754,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A43)</f>
@@ -2157,7 +2763,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A44)</f>
@@ -2166,7 +2772,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A45)</f>
@@ -2175,7 +2781,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A46)</f>

</xml_diff>

<commit_message>
formula: more math/trig functions
- SIGN
- SIN
- SINH
- SQRT
- SQRTPI
- SUM
- SUMPRODUCT
- SUMSQ
- TAN
- TANH
- TRUNC
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -217,6 +217,36 @@
   </si>
   <si>
     <t xml:space="preserve">SERIESSUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQRTPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUMPRODUCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUMSQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUNC</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -418,8 +448,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,9 +595,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,36 +1045,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AV46"/>
+  <dimension ref="A1:BF46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AV23" activeCellId="0" sqref="AV23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BD23" activeCellId="0" sqref="BD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="40" min="38" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="38" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="53" min="49" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="56" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,6 +1226,36 @@
       <c r="AV2" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="AW2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1375,6 +1441,46 @@
         <f aca="false">LEFT(SERIESSUM(AV18,0,2,AV19:AV22),7)</f>
         <v>0.69158</v>
       </c>
+      <c r="AW3" s="0" t="e">
+        <f aca="false">SIGN()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AX3" s="0" t="n">
+        <f aca="false">SIN(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AY3" s="0" t="str">
+        <f aca="false">LEFT(SINH(1),5)</f>
+        <v>1.175</v>
+      </c>
+      <c r="AZ3" s="0" t="e">
+        <f aca="false">SQRT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA3" s="0" t="n">
+        <f aca="false">SQRTPI(81/PI())</f>
+        <v>9</v>
+      </c>
+      <c r="BB3" s="0" t="n">
+        <f aca="false">SUMPRODUCT(AX23:AY24,AX26:AY27)</f>
+        <v>69</v>
+      </c>
+      <c r="BC3" s="0" t="n">
+        <f aca="false">SUMSQ(4)</f>
+        <v>16</v>
+      </c>
+      <c r="BD3" s="0" t="str">
+        <f aca="false">LEFT(TAN(45),6)</f>
+        <v>1.6197</v>
+      </c>
+      <c r="BE3" s="0" t="n">
+        <f aca="false">TANH(45)</f>
+        <v>1</v>
+      </c>
+      <c r="BF3" s="0" t="e">
+        <f aca="false">TRUNC()</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1560,6 +1666,38 @@
         <f aca="false">ROUNDUP(2.15,0)</f>
         <v>3</v>
       </c>
+      <c r="AW4" s="0" t="n">
+        <f aca="false">SIGN(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AX4" s="0" t="n">
+        <f aca="false">SIN(PI()/2)</f>
+        <v>1</v>
+      </c>
+      <c r="AY4" s="0" t="n">
+        <f aca="false">SINH(0)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="0" t="n">
+        <f aca="false">SQRT(4)</f>
+        <v>2</v>
+      </c>
+      <c r="BB4" s="0" t="n">
+        <f aca="false">SUMPRODUCT(1,2,3)</f>
+        <v>6</v>
+      </c>
+      <c r="BC4" s="0" t="n">
+        <f aca="false">SUMSQ(AX23:AY23)</f>
+        <v>5</v>
+      </c>
+      <c r="BE4" s="0" t="n">
+        <f aca="false">TANH(90)</f>
+        <v>1</v>
+      </c>
+      <c r="BF4" s="0" t="n">
+        <f aca="false">TRUNC(8.9)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1746,6 +1884,30 @@
         <f aca="false">ROUNDUP(2.15,1)</f>
         <v>2.2</v>
       </c>
+      <c r="AW5" s="0" t="n">
+        <f aca="false">SIGN(-1.2)</f>
+        <v>-1</v>
+      </c>
+      <c r="AZ5" s="0" t="n">
+        <f aca="false">SQRT(81)</f>
+        <v>9</v>
+      </c>
+      <c r="BB5" s="0" t="n">
+        <f aca="false">SUMPRODUCT(AX24:AY24,AX24:AY24)</f>
+        <v>25</v>
+      </c>
+      <c r="BC5" s="0" t="n">
+        <f aca="false">SUMSQ(AX23:AY24)</f>
+        <v>30</v>
+      </c>
+      <c r="BE5" s="0" t="str">
+        <f aca="false">LEFT(TANH(0.5),6)</f>
+        <v>0.4621</v>
+      </c>
+      <c r="BF5" s="0" t="n">
+        <f aca="false">TRUNC(-8.9)</f>
+        <v>-8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1920,6 +2082,22 @@
         <f aca="false">ROUNDUP(2.149,1)</f>
         <v>2.2</v>
       </c>
+      <c r="AW6" s="0" t="n">
+        <f aca="false">SIGN(1.321)</f>
+        <v>1</v>
+      </c>
+      <c r="AZ6" s="0" t="e">
+        <f aca="false">SQRT(-81)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB6" s="0" t="n">
+        <f aca="false">SUMPRODUCT(AX24:AY24,AX26:AY26,AX27:AY27)</f>
+        <v>314</v>
+      </c>
+      <c r="BF6" s="0" t="n">
+        <f aca="false">TRUNC(0.45)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2070,6 +2248,14 @@
         <f aca="false">ROUNDUP(-1.475,2)</f>
         <v>-1.48</v>
       </c>
+      <c r="AW7" s="0" t="e">
+        <f aca="false">SIGN("A")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BF7" s="0" t="n">
+        <f aca="false">TRUNC(1.23,2)</f>
+        <v>1.23</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2200,6 +2386,10 @@
         <f aca="false">ROUNDUP(21.5,-1)</f>
         <v>30</v>
       </c>
+      <c r="BF8" s="0" t="n">
+        <f aca="false">TRUNC(1.23,1)</f>
+        <v>1.2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2289,6 +2479,10 @@
         <f aca="false">ROUNDUP(626.3,-3)</f>
         <v>1000</v>
       </c>
+      <c r="BF9" s="0" t="n">
+        <f aca="false">TRUNC(-1.23,1)</f>
+        <v>-1.2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -2362,6 +2556,10 @@
         <f aca="false">ROUNDUP(1.98,-1)</f>
         <v>10</v>
       </c>
+      <c r="BF10" s="0" t="n">
+        <f aca="false">TRUNC(-1.23,4)</f>
+        <v>-1.23</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -2402,6 +2600,10 @@
       <c r="AU11" s="0" t="n">
         <f aca="false">ROUNDUP(-50.55,-2)</f>
         <v>-100</v>
+      </c>
+      <c r="BF11" s="0" t="n">
+        <f aca="false">TRUNC(1.23,-2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,6 +2643,10 @@
         <f aca="false">ROUNDUP(1.23,0)</f>
         <v>2</v>
       </c>
+      <c r="BF12" s="0" t="n">
+        <f aca="false">TRUNC(1.23,-5)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -2545,7 +2751,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="AR18" s="0" t="str">
         <f aca="false">ROMAN(999,4)</f>
@@ -2558,7 +2764,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="AR19" s="0" t="str">
         <f aca="false">ROMAN(699,1)</f>
@@ -2570,7 +2776,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="AR20" s="0" t="str">
         <f aca="false">ROMAN(699,2)</f>
@@ -2583,7 +2789,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="AR21" s="0" t="str">
         <f aca="false">ROMAN(699,3)</f>
@@ -2596,7 +2802,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="AR22" s="0" t="str">
         <f aca="false">ROMAN(699,4)</f>
@@ -2609,35 +2815,59 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="AX23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY23" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
+      </c>
+      <c r="AX24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY24" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F26" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A26)</f>
         <v>4</v>
       </c>
+      <c r="AX26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AY26" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A27)</f>
         <v>9</v>
       </c>
+      <c r="AX27" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AY27" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A28)</f>
@@ -2646,7 +2876,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A29)</f>
@@ -2655,7 +2885,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A30)</f>
@@ -2664,7 +2894,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F31" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A31)</f>
@@ -2673,7 +2903,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A33)</f>
@@ -2682,7 +2912,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A34)</f>
@@ -2691,7 +2921,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F35" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A35)</f>
@@ -2700,7 +2930,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F36" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A36)</f>
@@ -2709,7 +2939,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A37)</f>
@@ -2718,7 +2948,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F38" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A38)</f>
@@ -2727,7 +2957,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="F39" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A39)</f>
@@ -2736,7 +2966,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="F41" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A41)</f>
@@ -2745,7 +2975,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F42" s="0" t="e">
         <f aca="false">_xlfn.ARABIC(A42)</f>
@@ -2754,7 +2984,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F43" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A43)</f>
@@ -2763,7 +2993,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F44" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A44)</f>
@@ -2772,7 +3002,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F45" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A45)</f>
@@ -2781,7 +3011,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="F46" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A46)</f>

</xml_diff>

<commit_message>
formula: add support for text functions
- CHAR
- CLEAN
- CODE
- CONCATENATE
- EXACT
- LEFT
- LEN
- LOWER
- PROPER
- REPT
- RIGHT
- T
- TRIM
- UNICHAR
- UNICODE
- UPPER
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Logical" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Math and Trig" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Text" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -316,6 +317,63 @@
   </si>
   <si>
     <t xml:space="preserve">VM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONCATENATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
   </si>
 </sst>
 </file>
@@ -398,7 +456,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -420,6 +478,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,9 +510,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,10 +658,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,38 +1108,30 @@
   </sheetPr>
   <dimension ref="A1:BF46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="BD23" activeCellId="0" sqref="BD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="40" min="38" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="53" min="49" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="56" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3016,6 +3069,417 @@
       <c r="F46" s="0" t="n">
         <f aca="false">_xlfn.ARABIC(A46)</f>
         <v>995</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:P15"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.1938775510204"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="e">
+        <f aca="false">CHAR()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C3" s="0" t="e">
+        <f aca="false">CLEAN()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" s="0" t="e">
+        <f aca="false">CODE()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">CONCATENATE()</f>
+        <v/>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">EXACT("a","a")</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">LEFT(F3)</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="e">
+        <f aca="false">LEN()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" s="0" t="e">
+        <f aca="false">LOWER()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="0" t="e">
+        <f aca="false">PROPER()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="0" t="e">
+        <f aca="false">REPT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L3" s="0" t="e">
+        <f aca="false">T()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M3" s="0" t="e">
+        <f aca="false">TRIM()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N3" s="0" t="e">
+        <f aca="false">_xlfn.UNICHAR()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O3" s="0" t="e">
+        <f aca="false">CODE()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P3" s="0" t="e">
+        <f aca="false">UPPER()</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="str">
+        <f aca="false">CHAR(65)</f>
+        <v>A</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">CLEAN("")</f>
+        <v/>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">CODE("")</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="e">
+        <f aca="false">CONCATENATE(B14:C15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">EXACT("a","a ")</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">LEFT(D5,2)</f>
+        <v>33</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">LEN(1)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">LOWER("A")</f>
+        <v>a</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">PROPER("")</f>
+        <v/>
+      </c>
+      <c r="K4" s="0" t="e">
+        <f aca="false">REPT("")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">T(K6)</f>
+        <v>Foo</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">TRIM("A")</f>
+        <v>A</v>
+      </c>
+      <c r="N4" s="0" t="str">
+        <f aca="false">_xlfn.UNICHAR(32)</f>
+        <v> </v>
+      </c>
+      <c r="O4" s="0" t="e">
+        <f aca="false">_xlfn.UNICODE("")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P4" s="0" t="str">
+        <f aca="false">UPPER("A")</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="str">
+        <f aca="false">CHAR(33)</f>
+        <v>!</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">CLEAN(B4)</f>
+        <v>A</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">CODE(B5)</f>
+        <v>33</v>
+      </c>
+      <c r="E5" s="0" t="e">
+        <f aca="false">CONCATENATE(B14:C14)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">EXACT("b","b")</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">LEFT(D6,1)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">LEN(2)</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">LOWER("FOO")</f>
+        <v>foo</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">PROPER("foo bar")</f>
+        <v>Foo Bar</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">REPT("",0)</f>
+        <v/>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">T(H4)</f>
+        <v/>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">TRIM("A B")</f>
+        <v>A B</v>
+      </c>
+      <c r="N5" s="0" t="str">
+        <f aca="false">_xlfn.UNICHAR(66)</f>
+        <v>B</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">_xlfn.UNICODE(M5)</f>
+        <v>65</v>
+      </c>
+      <c r="P5" s="0" t="str">
+        <f aca="false">UPPER("a")</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="str">
+        <f aca="false">CHAR(90)</f>
+        <v>Z</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">CLEAN(CHAR(9)&amp;"foo"&amp;CHAR(10))</f>
+        <v>foo</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">CODE(C6)</f>
+        <v>102</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">CONCATENATE(B14,C14)</f>
+        <v>ab</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">EXACT(1,3)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">LEFT(C6,2)</f>
+        <v>fo</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">LEN(10)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">LOWER("foo")</f>
+        <v>foo</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">PROPER("foo")</f>
+        <v>Foo</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">REPT(J6,1)</f>
+        <v>Foo</v>
+      </c>
+      <c r="L6" s="0" t="e">
+        <f aca="false">T(J3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">TRIM("A  B")</f>
+        <v>A B</v>
+      </c>
+      <c r="O6" s="0" t="e">
+        <f aca="false">_xlfn.UNICODE(N6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P6" s="0" t="str">
+        <f aca="false">UPPER("foo bar baz")</f>
+        <v>FOO BAR BAZ</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="e">
+        <f aca="false">CHAR(256)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">CODE(C5)</f>
+        <v>65</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">EXACT(1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">LEN(C6)</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">PROPER("Foo")</f>
+        <v>Foo</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">REPT(J7,3)</f>
+        <v>FooFooFoo</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">TRIM(" A B C   D")</f>
+        <v>A B C D</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">_xlfn.UNICODE(N5)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="e">
+        <f aca="false">CHAR(-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">PROPER("foo bar baz   quuz")</f>
+        <v>Foo Bar Baz   Quuz</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">TRIM("A "&amp;CHAR(9)&amp;CHAR(9)&amp;" B  ")</f>
+        <v>A 		 B</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="str">
+        <f aca="false">CHAR(65.2)</f>
+        <v>A</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">PROPER("foo,bar,baz")</f>
+        <v>Foo,Bar,Baz</v>
+      </c>
+      <c r="K9" s="0" t="e">
+        <f aca="false">REPT(J7,-1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="str">
+        <f aca="false">CHAR(65.9)</f>
+        <v>A</v>
+      </c>
+      <c r="J10" s="0" t="str">
+        <f aca="false">PROPER("76BudGet")</f>
+        <v>76Budget</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formula: support for using named ranges/tables from formulas
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Logical" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Math and Trig" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Text" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Indexing" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -374,6 +375,9 @@
   </si>
   <si>
     <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDEX</t>
   </si>
 </sst>
 </file>
@@ -497,6 +501,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="FooBarNamedRange" displayName="FooBarNamedRange" ref="C5:D6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="a"/>
+    <tableColumn id="2" name="b"/>
+  </tableColumns>
+</table>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -510,10 +523,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,8 +670,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,24 +1128,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="38" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="53" min="47" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="55" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3089,18 +3107,22 @@
   </sheetPr>
   <dimension ref="B2:P15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P7" activeCellId="0" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,4 +3513,116 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B4:G14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">INDEX($C$5:$D$6,1,1)</f>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="0" t="str">
+        <f aca="false">INDEX($C$5:$D$6,2,1)</f>
+        <v>c</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="0" t="str">
+        <f aca="false">INDEX($C$5:$D$6,1,2)</f>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="0" t="str">
+        <f aca="false">INDEX($C$5:$D$6,2,2)</f>
+        <v>d</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="0" t="str">
+        <f aca="false">INDEX(C5:D5,1,1)</f>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="str">
+        <f aca="false">INDEX(D5:D6,2,1)</f>
+        <v>d</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="str">
+        <f aca="false">INDEX(FooBarNamedRange,1,1)</f>
+        <v>a</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formula: add more complex function support
- INDEX
- INDIRECT
- OFFSET
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t xml:space="preserve">INDEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDIRECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFFSET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B13</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1157,7 @@
     <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="53" min="47" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="55" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -3114,14 +3123,14 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -3520,22 +3529,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:G14"/>
+  <dimension ref="B4:H16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
@@ -3548,6 +3563,14 @@
         <f aca="false">INDEX($C$5:$D$6,1,1)</f>
         <v>a</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <f aca="true">INDIRECT("B13")</f>
+        <v>3</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="true">OFFSET(C5,1,1,1,1)</f>
+        <v>d</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
@@ -3559,6 +3582,14 @@
       <c r="F6" s="0" t="str">
         <f aca="false">INDEX($C$5:$D$6,2,1)</f>
         <v>c</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="true">INDIRECT(B16)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="true">OFFSET(C5,0,0,1,1)</f>
+        <v>a</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3566,18 +3597,34 @@
         <f aca="false">INDEX($C$5:$D$6,1,2)</f>
         <v>b</v>
       </c>
+      <c r="G7" s="0" t="e">
+        <f aca="false">INDIRECT()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="true">SUM(OFFSET(B13,0,0,2,2))</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F8" s="0" t="str">
         <f aca="false">INDEX($C$5:$D$6,2,2)</f>
         <v>d</v>
       </c>
+      <c r="H8" s="0" t="n">
+        <f aca="true">OFFSET(B13:D14,0,0,1,1)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="str">
         <f aca="false">INDEX(C5:D5,1,1)</f>
         <v>a</v>
       </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">OFFSET(FooBarNamedRange,0,0,1,1)</f>
+        <v>a</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="str">
@@ -3593,13 +3640,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,6 +3658,11 @@
       </c>
       <c r="D14" s="0" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formula: support for more statistical functions
- AVERAGE
- AVERAGEA
- COUNT
- COUNTA
- COUNTBLANK
- MEDIAN
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Math and Trig" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Text" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Indexing" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Statistics" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -387,6 +388,33 @@
   </si>
   <si>
     <t xml:space="preserve">B13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVERAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVERAGEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNTBLANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asd</t>
   </si>
 </sst>
 </file>
@@ -1156,9 +1184,7 @@
     <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="53" min="47" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="55" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,14 +3149,14 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
@@ -3531,14 +3557,14 @@
   </sheetPr>
   <dimension ref="B4:H16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3677,4 +3703,306 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="e">
+        <f aca="false">AVERAGE()</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">AVERAGEA(A2:C4)</f>
+        <v>5</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">COUNT()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">COUNTA()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="e">
+        <f aca="false">COUNTBLANK()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J2" s="0" t="e">
+        <f aca="false">MIN()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K2" s="0" t="e">
+        <f aca="false">MAX()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">MEDIAN(A2:C2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">AVERAGE(A2:C2)</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">AVERAGEA(0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">COUNT(A2:C2)</f>
+        <v>3</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">COUNTA(A2:C2)</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">COUNTBLANK(A3:C4)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">MIN(A2:C4)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">MAX(A3:C4)</f>
+        <v>9</v>
+      </c>
+      <c r="L3" s="0" t="e">
+        <f aca="false">MEDIAN()</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">AVERAGE(C2)</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="0" t="e">
+        <f aca="false">AVERAGEA()</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">COUNT(A3:C4)</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">COUNTA(A4:C5)</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">COUNTBLANK(A4:C6)</f>
+        <v>2</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">MIN(B3:C4)</f>
+        <v>4</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">MAX(A2:B3)</f>
+        <v>5</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">MEDIAN(A4)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">AVERAGE(A2:A4)</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f aca="false">AVERAGEA(A5:C5)</f>
+        <v>6</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">COUNT(A5:C5)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">COUNTA(A5:C6)</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">COUNTBLANK(A7:D9)</f>
+        <v>12</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">MIN(J6:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">MAX(K6:K9)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">MEDIAN(A3:C4)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">AVERAGE(A2:A5)</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">AVERAGE(B5:C6)</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">COUNT(A6:C6)</f>
+        <v>2</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">COUNTA(A7:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">MEDIAN(A2:C6)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="0" t="n">
+        <f aca="false">AVERAGE(C2:C5)</f>
+        <v>7</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <f aca="false">AVERAGEA(A5:C6)</f>
+        <v>3.25</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">COUNT(A1:C6)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="n">
+        <f aca="false">AVERAGE(B2:B5)</f>
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0" t="n">
+        <f aca="false">AVERAGE(B2:B4)</f>
+        <v>4.66666666666667</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="n">
+        <f aca="false">AVERAGE(A2:A6)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0" t="n">
+        <f aca="false">AVERAGE(A6:B6)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="0" t="n">
+        <f aca="false">AVERAGE(A6:C6)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formula: add more index functions
- HLOOKUP
- LOOKUP
- TRANSPOSE
- VLOOKUP
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="143">
   <si>
     <t xml:space="preserve">This sheet is used for unit testing of formulas.</t>
   </si>
@@ -387,7 +387,46 @@
     <t xml:space="preserve">OFFSET</t>
   </si>
   <si>
+    <t xml:space="preserve">VLOOKUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOOKUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLOOKUP</t>
+  </si>
+  <si>
     <t xml:space="preserve">B13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSPOSE</t>
   </si>
   <si>
     <t xml:space="preserve">AVERAGE</t>
@@ -560,9 +599,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,10 +747,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,26 +1203,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="34" min="30" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="40" min="38" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,16 +3182,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,16 +3584,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:H16"/>
+  <dimension ref="B4:K42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3577,6 +3611,15 @@
       <c r="H4" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
@@ -3597,6 +3640,18 @@
         <f aca="true">OFFSET(C5,1,1,1,1)</f>
         <v>d</v>
       </c>
+      <c r="I5" s="0" t="e">
+        <f aca="false">VLOOKUP()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J5" s="0" t="e">
+        <f aca="false">LOOKUP()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="0" t="e">
+        <f aca="false">HLOOKUP()</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
@@ -3616,6 +3671,18 @@
       <c r="H6" s="0" t="str">
         <f aca="true">OFFSET(C5,0,0,1,1)</f>
         <v>a</v>
+      </c>
+      <c r="I6" s="0" t="e">
+        <f aca="false">VLOOKUP(1,C18:E24)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J6" s="0" t="e">
+        <f aca="false">LOOKUP(1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="0" t="e">
+        <f aca="false">HLOOKUP(1)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,6 +3698,18 @@
         <f aca="true">SUM(OFFSET(B13,0,0,2,2))</f>
         <v>18</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">VLOOKUP(1,$C$18:$E$24,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">LOOKUP(1,C18:C24)</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">HLOOKUP(1,$C$27:$F$29,1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F8" s="0" t="str">
@@ -3641,6 +3720,18 @@
         <f aca="true">OFFSET(B13:D14,0,0,1,1)</f>
         <v>3</v>
       </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">VLOOKUP(1,$C$18:$E$24,2)</f>
+        <v>a</v>
+      </c>
+      <c r="J8" s="0" t="e">
+        <f aca="false">LOOKUP(2,C18:E18)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">HLOOKUP(1,$C$27:$F$29,2)</f>
+        <v>a</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="str">
@@ -3651,18 +3742,68 @@
         <f aca="false">OFFSET(FooBarNamedRange,0,0,1,1)</f>
         <v>a</v>
       </c>
+      <c r="I9" s="0" t="str">
+        <f aca="false">VLOOKUP(1,$C$18:$E$24,3)</f>
+        <v>h</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <f aca="false">LOOKUP(2,C19:E19)</f>
+        <v>2</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">HLOOKUP(1,$C$27:$F$29,3)</f>
+        <v>e</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="0" t="str">
         <f aca="false">INDEX(D5:D6,2,1)</f>
         <v>d</v>
       </c>
+      <c r="I10" s="0" t="e">
+        <f aca="false">VLOOKUP(2.3,$C$18:$E$24,1,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J10" s="0" t="str">
+        <f aca="false">LOOKUP(1,C18:C24,D18:D24)</f>
+        <v>a</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">HLOOKUP(1.5,$C$27:$F$29,1)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="0" t="str">
         <f aca="false">INDEX(FooBarNamedRange,1,1)</f>
         <v>a</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">VLOOKUP(2.3,$C$18:$E$24,1,TRUE())</f>
+        <v>2</v>
+      </c>
+      <c r="J11" s="0" t="str">
+        <f aca="false">LOOKUP(3,C18:C24,E18:E24)</f>
+        <v>j</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">HLOOKUP(1.5,$C$27:$F$29,1,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="0" t="n">
+        <f aca="false">VLOOKUP(4.2,C18:C24,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <f aca="false">LOOKUP("A",C18:E18,C19:E19)</f>
+        <v>b</v>
+      </c>
+      <c r="K12" s="0" t="e">
+        <f aca="false">HLOOKUP(1.5,$C$27:$F$29,1,0)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
@@ -3674,6 +3815,10 @@
       <c r="D13" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="I13" s="0" t="e">
+        <f aca="false">VLOOKUP(4.2,C19:C25,1,FALSE())</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
@@ -3686,9 +3831,249 @@
         <v>6</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="0" t="n">
+        <f aca="false">VLOOKUP(10,$C$18:$E$24,1)</f>
+        <v>7</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
+      </c>
+      <c r="I16" s="0" t="e">
+        <f aca="false">VLOOKUP(-1,$C$18:$E$24,1)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="0" t="str">
+        <f aca="false">VLOOKUP(10,$C$18:$E$24,2)</f>
+        <v>g</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="0" t="str">
+        <f aca="false">VLOOKUP(10,$C$18:$E$24,3)</f>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="0" t="e">
+        <f aca="false">VLOOKUP(10,$C$18:$E$24,4)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">VLOOKUP(10,$C$18:$E$24,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="0" t="e">
+        <f aca="false">VLOOKUP(10,$C$18:$E$24,0)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="0" t="str">
+        <f aca="false">VLOOKUP("CC",D18:E24,1)</f>
+        <v>c</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23" s="0" t="str">
+        <f aca="false">VLOOKUP("CC",D19:E25,2)</f>
+        <v>j</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="n">
+        <f aca="false" t="array" ref="C33:I33">TRANSPOSE(C18:C24)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="n">
+        <f aca="false" t="array" ref="C36:E38">TRANSPOSE(C27:E29)</f>
+        <v>1</v>
+      </c>
+      <c r="D36" s="0" t="str">
+        <v>a</v>
+      </c>
+      <c r="E36" s="0" t="str">
+        <v>e</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" s="0" t="str">
+        <v>b</v>
+      </c>
+      <c r="E37" s="0" t="str">
+        <v>f</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" s="0" t="str">
+        <v>c</v>
+      </c>
+      <c r="E38" s="0" t="str">
+        <v>g</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="0" t="n">
+        <f aca="false">C38</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="0" t="str">
+        <f aca="false">D37</f>
+        <v>b</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="n">
+        <f aca="false">D33</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3712,45 +4097,45 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E1" s="2" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,7 +4269,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>12</v>

</xml_diff>

<commit_message>
fixed IF and statistical functions
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D10" s="0" t="e">
         <f aca="false">IF(A5:A7,TRUE())</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="G10" s="0" t="e">
         <f aca="false">NOT(A6:A8)</f>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="D11" s="0" t="e">
         <f aca="false">IF(A8:A9,TRUE())</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="G11" s="0" t="e">
         <f aca="false">NOT(A7:A8)</f>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I12" s="0" t="e">
         <f aca="false">_xlfn.XOR(D11:D12)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,11 +4322,11 @@
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">AVERAGE(B5:C6)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">COUNT(A6:C6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">COUNTA(A7:D9)</f>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">MEDIAN(A2:C6)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">COUNT(A1:C6)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4366,19 +4366,19 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="0" t="n">
         <f aca="false">AVERAGE(A2:A6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="0" t="n">
         <f aca="false">AVERAGE(A6:B6)</f>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="0" t="n">
         <f aca="false">AVERAGE(A6:C6)</f>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel spreadsheet functions, part 3 (#351)
* fixed IF and statistical functions
* Issue #347
* DATETIME
* DAY, DAYS, Cells() fix
* MONTH
* MINUTE
* EDATE
* EOMONTH
</commit_message>
<xml_diff>
--- a/spreadsheet/formula/testdata/formulareference.xlsx
+++ b/spreadsheet/formula/testdata/formulareference.xlsx
@@ -1027,7 +1027,7 @@
       </c>
       <c r="D10" s="0" t="e">
         <f aca="false">IF(A5:A7,TRUE())</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="G10" s="0" t="e">
         <f aca="false">NOT(A6:A8)</f>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="D11" s="0" t="e">
         <f aca="false">IF(A8:A9,TRUE())</f>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="G11" s="0" t="e">
         <f aca="false">NOT(A7:A8)</f>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I12" s="0" t="e">
         <f aca="false">_xlfn.XOR(D11:D12)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,11 +4322,11 @@
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">AVERAGE(B5:C6)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">COUNT(A6:C6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">COUNTA(A7:D9)</f>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">MEDIAN(A2:C6)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">COUNT(A1:C6)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4366,19 +4366,19 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="0" t="n">
         <f aca="false">AVERAGE(A2:A6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="0" t="n">
         <f aca="false">AVERAGE(A6:B6)</f>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="0" t="n">
         <f aca="false">AVERAGE(A6:C6)</f>
-        <v>0.5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>